<commit_message>
Getting Login set up (not working, yet)
</commit_message>
<xml_diff>
--- a/crywolf/events.xlsx
+++ b/crywolf/events.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roden\ids-simulator\crywolf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761DDB5A-6747-498D-8FB0-82D48572F9A3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C10DA4CC-4BA4-426D-A476-E4F5B3435AD9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{62B91F44-AB14-4E8F-90E3-F7FB42A9F7C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{62B91F44-AB14-4E8F-90E3-F7FB42A9F7C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiple Country Auth" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,75 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Source IP</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <t>geoip_organization</t>
+  </si>
+  <si>
+    <t>geoip_country</t>
+  </si>
+  <si>
+    <t>geoip_city</t>
+  </si>
+  <si>
+    <t>geoip_region</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>doej@example.com</t>
+  </si>
+  <si>
+    <t>Success</t>
+  </si>
+  <si>
+    <t>2a00:1450:4864:20::328</t>
+  </si>
+  <si>
+    <t>o365</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -67,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -383,13 +447,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC9B28D-E5B3-4F98-ADC8-D7C2A600A333}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -435,7 +569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE3693BF-14FC-474F-886B-99BD5488BFB9}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>